<commit_message>
put .get in try catch
</commit_message>
<xml_diff>
--- a/Files/Succsess.xlsx
+++ b/Files/Succsess.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,1508 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1649350000</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Item no. 2002-511</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2721210000</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Item no. 2721-210/008-000</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2721120000</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Item no. 2721-120/008-000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2721110000</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Item no. 2721-110/008-000</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2694080000</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Item no. 285-191</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2694070000</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Item no. 285-194</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2694060000</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Item no. 285-195</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2694090000</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Item no. 285-197</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2694160000</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Item no. 285-184</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2694170000</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Item no. 285-187</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2694150000</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Item no. 285-181</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2694180000</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Item no. 285-188</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2663340000</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Item no. 285-144</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2663350000</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Item no. 285-147</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2663260000</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Item no. 285-154</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2663250000</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Item no. 285-150</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2663330000</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Item no. 285-141</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2663270000</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Item no. 285-151</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2663280000</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Item no. 285-157</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2663290000</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Item no. 285-159</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2663360000</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Item no. 285-148</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2663400000</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Item no. 285-450</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2486490000</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Item no. 855-2701/035-001</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2473420000</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Item no. 2626-1101</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2500220000</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Item no. 250-220/000-012</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2562660000</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Item no. 285-430</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2556160000</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Item no. 255-616/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2565240000</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Item no. 256-524/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2566020000</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Item no. 256-602/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2566030000</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Item no. 256-603/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2566040000</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Item no. 256-604/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2566050000</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Item no. 256-605/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2566060000</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Item no. 256-606/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2566070000</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Item no. 256-607/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2566080000</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Item no. 256-608/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2574240000</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Item no. 257-424/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2581280000</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Item no. 2002-2234</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2576240000</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Item no. 257-624/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2576160000</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Item no. 257-616/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2576070000</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Item no. 257-607/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2576050000</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Item no. 257-605/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2576100000</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Item no. 257-610/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2576080000</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Item no. 257-608/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2576090000</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Item no. 257-609/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2576030000</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Item no. 257-603/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2576120000</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Item no. 257-612/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2576040000</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Item no. 257-604/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2576020000</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Item no. 257-602/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2579620000</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Item no. 2000-5311</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2579610000</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Item no. 2000-5311</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2473100000</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Item no. 2626-1112/020-000</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2473080000</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Item no. 2626-1110/020-000</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2473060000</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Item no. 2626-1108/020-000</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2473040000</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Item no. 2626-1106/020-000</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2473030000</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Item no. 2626-1105/020-000</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2473050000</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Item no. 2626-1107/020-000</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2473020000</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Item no. 2626-1104/020-000</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2473010000</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Item no. 2626-1103/020-000</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2473000000</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Item no. 2626-1102/020-000</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>2551530000</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Item no. 285-131</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2583170000</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Item no. 285-427</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>2583090000</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Item no. 285-427</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>2583180000</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Item no. 285-427</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>2634950000</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Item no. 285-435</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>2552100000</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Item no. 285-135</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>2552110000</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Item no. 285-135</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>2551540000</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Item no. 285-139</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>2552130000</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Item no. 285-135</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>2552120000</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Item no. 285-135</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>2552140000</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Item no. 285-135</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>2661280000</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Item no. 249-116</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>2618110000</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Item no. 857-364</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>2618050000</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Item no. 857-358</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>2618020000</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Item no. 857-304</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>2618010000</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Item no. 857-357</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>2618150000</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Item no. 857-357</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>2617840000</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Item no. 857-357</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>2617850000</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Item no. 857-358/006-000</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>2617860000</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Item no. 857-303</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>2617870000</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Item no. 857-359</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>2617890000</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Item no. 857-359</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>2617900000</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Item no. 857-357</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>2617950000</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Item no. 857-368/006-000</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>2618070000</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Item no. 857-369</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>2618160000</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Item no. 857-364</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>2618140000</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Item no. 857-359</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>2618170000</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Item no. 857-369</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2618210000</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Item no. 857-368</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2618240000</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Item no. 857-359</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2618180000</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Item no. 857-303</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>2564360000</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Item no. 256-436/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>2566090000</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Item no. 256-609/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>2566100000</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Item no. 256-610/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>2556010000</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Item no. 855-2701/064-001</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>2556020000</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Item no. 255-602/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>2556030000</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Item no. 255-603/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>2556040000</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Item no. 255-604/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>2581250000</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Item no. 2002-2231</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>2576060000</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Item no. 257-606/000-009/999-950</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>